<commit_message>
went through Programming, found some minor mistakes
there are more mistakes to be found, not urgent
</commit_message>
<xml_diff>
--- a/Map2Hex.xlsx
+++ b/Map2Hex.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bw_\Documents\AAU\P3\gitkraken\testLTC\testLTC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bw_\Documents\AAU\P3\gitkraken\testLTC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -488,7 +488,7 @@
   <dimension ref="B2:AJ16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AE18" sqref="AE18"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,7 +595,7 @@
         <v>128</v>
       </c>
       <c r="N3" s="5">
-        <f t="shared" ref="N3:O3" si="0">D3</f>
+        <f t="shared" ref="N3" si="0">D3</f>
         <v>1</v>
       </c>
       <c r="O3" s="5">
@@ -702,14 +702,14 @@
       <c r="AD4" s="5"/>
       <c r="AE4" s="5" t="str">
         <f>DEC2HEX(SUM(Q3:S5))</f>
-        <v>A5</v>
+        <v>81</v>
       </c>
       <c r="AF4" s="5"/>
       <c r="AG4" s="5"/>
       <c r="AH4" s="5"/>
       <c r="AI4" s="5" t="str">
         <f>DEC2HEX(SUM(U3:W5))</f>
-        <v>F7</v>
+        <v>B7</v>
       </c>
       <c r="AJ4" s="6"/>
     </row>
@@ -722,12 +722,8 @@
         <v>1</v>
       </c>
       <c r="E5" s="5"/>
-      <c r="F5" s="5">
-        <v>1</v>
-      </c>
-      <c r="G5" s="5">
-        <v>1</v>
-      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
       <c r="H5" s="5">
         <v>1</v>
       </c>
@@ -755,16 +751,16 @@
       </c>
       <c r="R5" s="5">
         <f>F5*4</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="S5" s="5">
         <f>G5*32</f>
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="T5" s="5"/>
       <c r="U5" s="5">
         <f>G5*64</f>
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="V5" s="5">
         <f>H5*4</f>
@@ -841,12 +837,8 @@
         <v>1</v>
       </c>
       <c r="E7" s="5"/>
-      <c r="F7" s="5">
-        <v>1</v>
-      </c>
-      <c r="G7" s="5">
-        <v>1</v>
-      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
       <c r="H7" s="5">
         <v>1</v>
       </c>
@@ -874,16 +866,16 @@
       </c>
       <c r="R7" s="5">
         <f>F5</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S7" s="5">
         <f>G5*16</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="T7" s="5"/>
       <c r="U7" s="5">
         <f>G5*128</f>
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="V7" s="5">
         <f>H5</f>
@@ -967,14 +959,14 @@
       <c r="AD8" s="5"/>
       <c r="AE8" s="5" t="str">
         <f>DEC2HEX(SUM(Q7:S9))</f>
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="AF8" s="5"/>
       <c r="AG8" s="5"/>
       <c r="AH8" s="5"/>
       <c r="AI8" s="5" t="str">
         <f>DEC2HEX(SUM(U7:W9))</f>
-        <v>F7</v>
+        <v>37</v>
       </c>
       <c r="AJ8" s="6"/>
     </row>
@@ -1022,16 +1014,16 @@
       </c>
       <c r="R9" s="5">
         <f>F7*4</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="S9" s="5">
         <f>G7*32</f>
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="T9" s="5"/>
       <c r="U9" s="5">
         <f>G7*64</f>
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="V9" s="5">
         <f>H7*4</f>
@@ -1119,16 +1111,16 @@
       </c>
       <c r="R11" s="5">
         <f>F7</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S11" s="5">
         <f>G7*16</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="T11" s="5"/>
       <c r="U11" s="5">
         <f>G7*128</f>
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="V11" s="5">
         <f>H7</f>
@@ -1202,14 +1194,14 @@
       <c r="AD12" s="5"/>
       <c r="AE12" s="5" t="str">
         <f>DEC2HEX(SUM(Q11:S13))</f>
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="AF12" s="5"/>
       <c r="AG12" s="5"/>
       <c r="AH12" s="5"/>
       <c r="AI12" s="5" t="str">
         <f>DEC2HEX(SUM(U11:W13))</f>
-        <v>F7</v>
+        <v>77</v>
       </c>
       <c r="AJ12" s="6"/>
     </row>

</xml_diff>